<commit_message>
Pricesheet for Mon 08 Feb 2021 22:07:23 CAT
</commit_message>
<xml_diff>
--- a/pricesheets/08-02-2021.xlsx
+++ b/pricesheets/08-02-2021.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="189">
   <si>
     <t>Company Name</t>
   </si>
@@ -181,19 +181,19 @@
     <t>24.0000</t>
   </si>
   <si>
-    <t>1.4346</t>
-  </si>
-  <si>
-    <t>5.0000</t>
-  </si>
-  <si>
-    <t>2.2383</t>
-  </si>
-  <si>
-    <t>17.3482</t>
-  </si>
-  <si>
-    <t>4.2907</t>
+    <t>1.6347</t>
+  </si>
+  <si>
+    <t>5.4141</t>
+  </si>
+  <si>
+    <t>2.2517</t>
+  </si>
+  <si>
+    <t>17.5792</t>
+  </si>
+  <si>
+    <t>4.4482</t>
   </si>
   <si>
     <t>873.3333</t>
@@ -202,370 +202,385 @@
     <t>80.0000</t>
   </si>
   <si>
-    <t>10.6720</t>
-  </si>
-  <si>
-    <t>102.5459</t>
-  </si>
-  <si>
-    <t>20.5000</t>
-  </si>
-  <si>
-    <t>0.4125</t>
-  </si>
-  <si>
-    <t>44.5097</t>
-  </si>
-  <si>
-    <t>14.7805</t>
-  </si>
-  <si>
-    <t>1.1500</t>
-  </si>
-  <si>
-    <t>24.8553</t>
+    <t>11.6751</t>
+  </si>
+  <si>
+    <t>92.3950</t>
+  </si>
+  <si>
+    <t>21.0000</t>
+  </si>
+  <si>
+    <t>0.4033</t>
+  </si>
+  <si>
+    <t>47.2089</t>
+  </si>
+  <si>
+    <t>16.6370</t>
+  </si>
+  <si>
+    <t>1.3800</t>
+  </si>
+  <si>
+    <t>25.5416</t>
   </si>
   <si>
     <t>2.2000</t>
   </si>
   <si>
-    <t>1.9444</t>
-  </si>
-  <si>
-    <t>12.5374</t>
+    <t>1.9431</t>
+  </si>
+  <si>
+    <t>13.5233</t>
   </si>
   <si>
     <t>5.5000</t>
   </si>
   <si>
+    <t>0.2496</t>
+  </si>
+  <si>
+    <t>0.2590</t>
+  </si>
+  <si>
+    <t>100.0000</t>
+  </si>
+  <si>
+    <t>58.8677</t>
+  </si>
+  <si>
+    <t>18.8000</t>
+  </si>
+  <si>
+    <t>1.0500</t>
+  </si>
+  <si>
+    <t>16.0000</t>
+  </si>
+  <si>
+    <t>0.0740</t>
+  </si>
+  <si>
+    <t>40.9670</t>
+  </si>
+  <si>
+    <t>4.1088</t>
+  </si>
+  <si>
+    <t>72.1000</t>
+  </si>
+  <si>
+    <t>0.2745</t>
+  </si>
+  <si>
+    <t>6.0469</t>
+  </si>
+  <si>
+    <t>18.5000</t>
+  </si>
+  <si>
+    <t>33.4646</t>
+  </si>
+  <si>
+    <t>23.8500</t>
+  </si>
+  <si>
+    <t>1.7500</t>
+  </si>
+  <si>
+    <t>15.6000</t>
+  </si>
+  <si>
+    <t>35.3165</t>
+  </si>
+  <si>
+    <t>22.6995</t>
+  </si>
+  <si>
+    <t>0.3444</t>
+  </si>
+  <si>
+    <t>0.8026</t>
+  </si>
+  <si>
+    <t>45.6464</t>
+  </si>
+  <si>
+    <t>0.9000</t>
+  </si>
+  <si>
+    <t>1.1425</t>
+  </si>
+  <si>
+    <t>0.4173</t>
+  </si>
+  <si>
+    <t>40.0000</t>
+  </si>
+  <si>
+    <t>0.0002</t>
+  </si>
+  <si>
+    <t>0.9800</t>
+  </si>
+  <si>
+    <t>8.6000</t>
+  </si>
+  <si>
+    <t>2.6421</t>
+  </si>
+  <si>
+    <t>Closing Price</t>
+  </si>
+  <si>
+    <t>26.5000</t>
+  </si>
+  <si>
+    <t>1.6689</t>
+  </si>
+  <si>
+    <t>5.9509</t>
+  </si>
+  <si>
+    <t>2.2543</t>
+  </si>
+  <si>
+    <t>17.5000</t>
+  </si>
+  <si>
+    <t>4.5552</t>
+  </si>
+  <si>
+    <t>875.0000</t>
+  </si>
+  <si>
+    <t>12.0727</t>
+  </si>
+  <si>
+    <t>90.2500</t>
+  </si>
+  <si>
+    <t>0.3999</t>
+  </si>
+  <si>
+    <t>47.9970</t>
+  </si>
+  <si>
+    <t>19.7532</t>
+  </si>
+  <si>
+    <t>1.6500</t>
+  </si>
+  <si>
+    <t>1.9457</t>
+  </si>
+  <si>
+    <t>16.1997</t>
+  </si>
+  <si>
+    <t>6.0000</t>
+  </si>
+  <si>
     <t>0.2500</t>
   </si>
   <si>
-    <t>0.2590</t>
-  </si>
-  <si>
-    <t>101.4206</t>
-  </si>
-  <si>
-    <t>58.2500</t>
-  </si>
-  <si>
-    <t>15.7000</t>
-  </si>
-  <si>
-    <t>0.9742</t>
-  </si>
-  <si>
-    <t>16.3000</t>
-  </si>
-  <si>
-    <t>0.0737</t>
-  </si>
-  <si>
-    <t>41.0464</t>
-  </si>
-  <si>
-    <t>3.6600</t>
-  </si>
-  <si>
-    <t>72.1000</t>
-  </si>
-  <si>
-    <t>0.2745</t>
-  </si>
-  <si>
-    <t>6.1199</t>
-  </si>
-  <si>
-    <t>16.3506</t>
-  </si>
-  <si>
-    <t>30.0499</t>
-  </si>
-  <si>
-    <t>19.9000</t>
-  </si>
-  <si>
-    <t>1.7500</t>
-  </si>
-  <si>
-    <t>15.6000</t>
-  </si>
-  <si>
-    <t>29.8400</t>
-  </si>
-  <si>
-    <t>20.2995</t>
-  </si>
-  <si>
-    <t>0.3156</t>
-  </si>
-  <si>
-    <t>0.7497</t>
-  </si>
-  <si>
-    <t>46.0984</t>
-  </si>
-  <si>
-    <t>0.9000</t>
-  </si>
-  <si>
-    <t>0.9525</t>
-  </si>
-  <si>
-    <t>0.3885</t>
-  </si>
-  <si>
-    <t>40.0000</t>
-  </si>
-  <si>
-    <t>0.0002</t>
-  </si>
-  <si>
-    <t>0.9800</t>
-  </si>
-  <si>
-    <t>7.3409</t>
-  </si>
-  <si>
-    <t>2.6900</t>
-  </si>
-  <si>
-    <t>Closing Price</t>
-  </si>
-  <si>
-    <t>1.6347</t>
-  </si>
-  <si>
-    <t>5.4141</t>
-  </si>
-  <si>
-    <t>2.2517</t>
-  </si>
-  <si>
-    <t>17.5792</t>
-  </si>
-  <si>
-    <t>4.4482</t>
-  </si>
-  <si>
-    <t>11.6751</t>
-  </si>
-  <si>
-    <t>92.3950</t>
-  </si>
-  <si>
-    <t>20.8069</t>
-  </si>
-  <si>
-    <t>0.4033</t>
-  </si>
-  <si>
-    <t>47.2089</t>
-  </si>
-  <si>
-    <t>16.6370</t>
-  </si>
-  <si>
-    <t>1.3800</t>
-  </si>
-  <si>
-    <t>25.5416</t>
-  </si>
-  <si>
-    <t>1.9431</t>
-  </si>
-  <si>
-    <t>13.5233</t>
-  </si>
-  <si>
-    <t>0.2496</t>
-  </si>
-  <si>
-    <t>100.0000</t>
-  </si>
-  <si>
-    <t>58.8677</t>
-  </si>
-  <si>
-    <t>18.8000</t>
-  </si>
-  <si>
-    <t>1.0500</t>
-  </si>
-  <si>
-    <t>16.0000</t>
-  </si>
-  <si>
-    <t>0.0740</t>
-  </si>
-  <si>
-    <t>40.9670</t>
-  </si>
-  <si>
-    <t>4.1088</t>
-  </si>
-  <si>
-    <t>6.0469</t>
-  </si>
-  <si>
-    <t>17.5901</t>
-  </si>
-  <si>
-    <t>33.4646</t>
-  </si>
-  <si>
-    <t>23.8500</t>
-  </si>
-  <si>
-    <t>35.3165</t>
-  </si>
-  <si>
-    <t>22.6995</t>
-  </si>
-  <si>
-    <t>0.3445</t>
-  </si>
-  <si>
-    <t>0.8026</t>
-  </si>
-  <si>
-    <t>45.6464</t>
-  </si>
-  <si>
-    <t>1.1425</t>
-  </si>
-  <si>
-    <t>0.4173</t>
-  </si>
-  <si>
-    <t>8.6000</t>
-  </si>
-  <si>
-    <t>2.6421</t>
+    <t>0.3105</t>
+  </si>
+  <si>
+    <t>59.7426</t>
+  </si>
+  <si>
+    <t>1.1601</t>
+  </si>
+  <si>
+    <t>16.8800</t>
+  </si>
+  <si>
+    <t>0.0700</t>
+  </si>
+  <si>
+    <t>43.5294</t>
+  </si>
+  <si>
+    <t>4.6222</t>
+  </si>
+  <si>
+    <t>6.1300</t>
+  </si>
+  <si>
+    <t>18.5866</t>
+  </si>
+  <si>
+    <t>33.3214</t>
+  </si>
+  <si>
+    <t>24.0013</t>
+  </si>
+  <si>
+    <t>1.8206</t>
+  </si>
+  <si>
+    <t>17.8868</t>
+  </si>
+  <si>
+    <t>36.0000</t>
+  </si>
+  <si>
+    <t>23.8905</t>
+  </si>
+  <si>
+    <t>0.3605</t>
+  </si>
+  <si>
+    <t>0.8698</t>
+  </si>
+  <si>
+    <t>45.7864</t>
+  </si>
+  <si>
+    <t>0.9200</t>
+  </si>
+  <si>
+    <t>1.2875</t>
+  </si>
+  <si>
+    <t>0.4903</t>
+  </si>
+  <si>
+    <t>2.5061</t>
   </si>
   <si>
     <t>Total Traded Volume</t>
   </si>
   <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>2800</t>
+  </si>
+  <si>
+    <t>5500</t>
+  </si>
+  <si>
+    <t>191600</t>
+  </si>
+  <si>
+    <t>15000</t>
+  </si>
+  <si>
+    <t>35500</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>98100</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>6100</t>
+  </si>
+  <si>
+    <t>16000</t>
+  </si>
+  <si>
+    <t>238800</t>
+  </si>
+  <si>
+    <t>2502500</t>
+  </si>
+  <si>
+    <t>6900</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
-    <t>39900</t>
-  </si>
-  <si>
-    <t>25600</t>
-  </si>
-  <si>
-    <t>102800</t>
-  </si>
-  <si>
-    <t>1200</t>
-  </si>
-  <si>
-    <t>74400</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>434000</t>
-  </si>
-  <si>
-    <t>24100</t>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>390900</t>
+  </si>
+  <si>
+    <t>6700</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>14800</t>
+  </si>
+  <si>
+    <t>281100</t>
+  </si>
+  <si>
+    <t>181300</t>
+  </si>
+  <si>
+    <t>2500</t>
+  </si>
+  <si>
+    <t>3527200</t>
+  </si>
+  <si>
+    <t>3400</t>
+  </si>
+  <si>
+    <t>73400</t>
+  </si>
+  <si>
+    <t>4600</t>
+  </si>
+  <si>
+    <t>932600</t>
+  </si>
+  <si>
+    <t>81200</t>
+  </si>
+  <si>
+    <t>300000</t>
+  </si>
+  <si>
+    <t>1700</t>
+  </si>
+  <si>
+    <t>10600</t>
+  </si>
+  <si>
+    <t>24900</t>
+  </si>
+  <si>
+    <t>46500</t>
+  </si>
+  <si>
+    <t>729500</t>
+  </si>
+  <si>
+    <t>17800</t>
+  </si>
+  <si>
+    <t>135300</t>
+  </si>
+  <si>
+    <t>10800</t>
+  </si>
+  <si>
+    <t>41300</t>
   </si>
   <si>
     <t>18300</t>
   </si>
   <si>
-    <t>15800</t>
-  </si>
-  <si>
-    <t>801000</t>
-  </si>
-  <si>
-    <t>20000</t>
-  </si>
-  <si>
-    <t>171800</t>
-  </si>
-  <si>
-    <t>73900</t>
-  </si>
-  <si>
-    <t>259300</t>
-  </si>
-  <si>
-    <t>900</t>
-  </si>
-  <si>
-    <t>45100</t>
-  </si>
-  <si>
-    <t>17300</t>
-  </si>
-  <si>
-    <t>494900</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>683900</t>
-  </si>
-  <si>
-    <t>511600</t>
-  </si>
-  <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>12900</t>
-  </si>
-  <si>
-    <t>51500</t>
-  </si>
-  <si>
-    <t>736400</t>
-  </si>
-  <si>
-    <t>45200</t>
-  </si>
-  <si>
-    <t>1700</t>
-  </si>
-  <si>
-    <t>4400</t>
-  </si>
-  <si>
-    <t>230300</t>
-  </si>
-  <si>
-    <t>37500</t>
-  </si>
-  <si>
-    <t>1104600</t>
-  </si>
-  <si>
-    <t>2700</t>
-  </si>
-  <si>
-    <t>326400</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>51300</t>
-  </si>
-  <si>
-    <t>100500</t>
-  </si>
-  <si>
     <t>200</t>
   </si>
   <si>
-    <t>21500</t>
+    <t>297300</t>
   </si>
 </sst>
 </file>
@@ -923,7 +938,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -954,726 +969,726 @@
         <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
         <v>106</v>
       </c>
       <c r="D6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
         <v>107</v>
       </c>
       <c r="D7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
         <v>108</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
         <v>109</v>
       </c>
       <c r="D9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
         <v>110</v>
       </c>
       <c r="D10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="D11" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>112</v>
       </c>
       <c r="D12" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D14" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D15" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
         <v>115</v>
       </c>
       <c r="D17" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
         <v>116</v>
       </c>
       <c r="D18" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
         <v>117</v>
       </c>
       <c r="D19" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
         <v>118</v>
       </c>
       <c r="D20" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D23" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="D24" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
         <v>121</v>
       </c>
       <c r="D25" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="D26" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D27" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
         <v>124</v>
       </c>
       <c r="D29" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>78</v>
       </c>
       <c r="D30" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D31" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D32" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D33" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D34" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="D35" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D36" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C37" t="s">
-        <v>130</v>
+        <v>85</v>
       </c>
       <c r="D37" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D38" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D39" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D40" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
       <c r="D41" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C42" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="D42" t="s">
-        <v>144</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C43" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D43" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C44" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D44" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C45" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D45" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C46" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D46" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C47" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D47" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C48" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
       <c r="D48" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C49" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D49" t="s">
-        <v>179</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C50" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D50" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C51" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="D51" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D52" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D53" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C54" t="s">
-        <v>141</v>
+        <v>102</v>
       </c>
       <c r="D54" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" t="s">
+        <v>103</v>
+      </c>
+      <c r="D55" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
         <v>52</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>104</v>
       </c>
-      <c r="C55" t="s">
-        <v>142</v>
-      </c>
-      <c r="D55" t="s">
-        <v>183</v>
+      <c r="C56" t="s">
+        <v>144</v>
+      </c>
+      <c r="D56" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>